<commit_message>
boosted regression tree - re-organize & new for all plant species richness
</commit_message>
<xml_diff>
--- a/BRT/boosted regression trees 08-12-2014.xlsx
+++ b/BRT/boosted regression trees 08-12-2014.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$165</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$201</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="39">
   <si>
     <t>FP richness</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>GIS-DERIVED</t>
+  </si>
+  <si>
+    <t>All plant richness</t>
   </si>
 </sst>
 </file>
@@ -571,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C165"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A139" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1916,16 +1919,293 @@
         <v>35</v>
       </c>
     </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B167" s="7"/>
+      <c r="C167" s="7"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B170" s="4">
+        <v>50.141071009999997</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" s="4">
+        <v>19.668259450000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B172" s="4">
+        <v>6.7384688600000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B173" s="4">
+        <v>6.1890596499999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" s="4">
+        <v>5.6525875799999996</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B175" s="4">
+        <v>2.8722203999999998</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B176" s="4">
+        <v>2.31918523</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B177" s="4">
+        <v>1.5034017200000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B178" s="4">
+        <v>1.2325731499999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B179" s="4">
+        <v>0.90205245000000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B180" s="4">
+        <v>0.65937913999999997</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B181" s="4">
+        <v>0.47221640999999998</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B182" s="4">
+        <v>0.38907717000000003</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B183" s="4">
+        <v>0.363954</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B184" s="4">
+        <v>0.28998081999999997</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B185" s="4">
+        <v>0.26705433000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B186" s="4">
+        <v>0.22551354000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B187" s="4">
+        <v>9.3602989999999997E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B188" s="4">
+        <v>1.2970809999999999E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B189" s="4">
+        <v>7.3712700000000001E-3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="8"/>
+      <c r="B190" s="8"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B191" s="4">
+        <v>863.52110000000005</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B192" s="4">
+        <v>374.85719999999998</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="10"/>
+      <c r="B193" s="8"/>
+    </row>
+    <row r="194" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A194" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B194" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C194" s="12">
+        <f>(B191-B192)/B191*100</f>
+        <v>56.589688427995569</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="2"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C197" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C198" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B201" s="8"/>
+      <c r="C201" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;F</oddFooter>
   </headerFooter>
-  <rowBreaks count="3" manualBreakCount="3">
+  <rowBreaks count="4" manualBreakCount="4">
     <brk id="41" max="16383" man="1"/>
     <brk id="85" max="16383" man="1"/>
     <brk id="125" max="16383" man="1"/>
+    <brk id="166" max="3" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>